<commit_message>
Updated results excel (x264 and leela)
</commit_message>
<xml_diff>
--- a/results/results_table.xlsx
+++ b/results/results_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max/Desktop/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{CAA2AF3B-0A18-7C4C-9546-9DE8C7D0CAEB}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{49DC639F-604F-A34A-9D80-939772D3C1BA}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="4" xr2:uid="{4BDD7C24-A808-BD4F-9094-4693B707796C}"/>
   </bookViews>
@@ -169,7 +169,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -192,11 +192,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -218,6 +231,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -536,7 +558,7 @@
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3161,7 +3183,7 @@
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3364,15 +3386,27 @@
       <c r="A8" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
+      <c r="B8" s="5">
+        <v>107510874570</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="10">
+        <v>107509988030</v>
+      </c>
+      <c r="E8" s="5">
+        <v>107509744250</v>
+      </c>
+      <c r="F8" s="5">
+        <v>107512107830</v>
+      </c>
+      <c r="G8" s="5">
+        <v>107509744320</v>
+      </c>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
-      <c r="J8" s="7"/>
+      <c r="J8" s="7">
+        <v>107509744250</v>
+      </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
       <c r="M8" s="5"/>
@@ -3383,15 +3417,733 @@
       <c r="A9" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
+      <c r="B9" s="5">
+        <v>2439482</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="10">
+        <v>2439481</v>
+      </c>
+      <c r="E9" s="5">
+        <v>2439481</v>
+      </c>
+      <c r="F9" s="5">
+        <v>2439482</v>
+      </c>
+      <c r="G9" s="5">
+        <v>2439480</v>
+      </c>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
-      <c r="J9" s="7"/>
+      <c r="J9" s="7">
+        <v>2437132</v>
+      </c>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" s="3"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="3"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="5">
+        <v>477</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="11">
+        <v>392</v>
+      </c>
+      <c r="E11" s="5">
+        <v>397</v>
+      </c>
+      <c r="F11" s="5">
+        <v>476</v>
+      </c>
+      <c r="G11" s="5">
+        <v>397</v>
+      </c>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5">
+        <v>395</v>
+      </c>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="6">
+        <v>7</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="12">
+        <v>7</v>
+      </c>
+      <c r="E12" s="4">
+        <v>7</v>
+      </c>
+      <c r="F12" s="4">
+        <v>7</v>
+      </c>
+      <c r="G12" s="4">
+        <v>7</v>
+      </c>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4">
+        <v>7</v>
+      </c>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13" s="3"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="3"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="5">
+        <v>17092299</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="10">
+        <v>17091385</v>
+      </c>
+      <c r="E14" s="5">
+        <v>17093605</v>
+      </c>
+      <c r="F14" s="5">
+        <v>17091391</v>
+      </c>
+      <c r="G14" s="5">
+        <v>17093773</v>
+      </c>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="7">
+        <v>17097085</v>
+      </c>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="5">
+        <v>46677946</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="10">
+        <v>46670597</v>
+      </c>
+      <c r="E15" s="5">
+        <v>46859891</v>
+      </c>
+      <c r="F15" s="5">
+        <v>46658671</v>
+      </c>
+      <c r="G15" s="5">
+        <v>46824043</v>
+      </c>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="7">
+        <v>4689511</v>
+      </c>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="5">
+        <v>63770245</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="10">
+        <v>63761982</v>
+      </c>
+      <c r="E16" s="5">
+        <v>63953496</v>
+      </c>
+      <c r="F16" s="5">
+        <v>63750062</v>
+      </c>
+      <c r="G16" s="5">
+        <v>63917816</v>
+      </c>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="7">
+        <v>21786596</v>
+      </c>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A17" s="3"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="3"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="5">
+        <v>63803013</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="10">
+        <v>63794750</v>
+      </c>
+      <c r="E18" s="5">
+        <v>63986264</v>
+      </c>
+      <c r="F18" s="5">
+        <v>63782830</v>
+      </c>
+      <c r="G18" s="5">
+        <v>63950584</v>
+      </c>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="7">
+        <v>64023257</v>
+      </c>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="5">
+        <v>107447071560</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="10">
+        <v>107446193280</v>
+      </c>
+      <c r="E19" s="5">
+        <v>107445757990</v>
+      </c>
+      <c r="F19" s="5">
+        <v>107448325000</v>
+      </c>
+      <c r="G19" s="5">
+        <v>107445793730</v>
+      </c>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="7">
+        <v>107445721000</v>
+      </c>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="5">
+        <v>86841438458</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="10">
+        <v>86840995346</v>
+      </c>
+      <c r="E20" s="5">
+        <v>86840873422</v>
+      </c>
+      <c r="F20" s="5">
+        <v>86842055119</v>
+      </c>
+      <c r="G20" s="5">
+        <v>86840873487</v>
+      </c>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="7">
+        <v>86840873425</v>
+      </c>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="5">
+        <v>20669436113</v>
+      </c>
+      <c r="C21" s="3"/>
+      <c r="D21" s="10">
+        <v>20668992688</v>
+      </c>
+      <c r="E21" s="5">
+        <v>20668870829</v>
+      </c>
+      <c r="F21" s="5">
+        <v>20670052709</v>
+      </c>
+      <c r="G21" s="5">
+        <v>20668870829</v>
+      </c>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="7">
+        <v>20668870829</v>
+      </c>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A22" s="3"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="3"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="5">
+        <v>49998363</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="D23" s="10">
+        <v>54659042</v>
+      </c>
+      <c r="E23" s="5">
+        <v>55995617</v>
+      </c>
+      <c r="F23" s="5">
+        <v>56179259</v>
+      </c>
+      <c r="G23" s="5">
+        <v>58411091</v>
+      </c>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="7">
+        <v>51663151</v>
+      </c>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" s="5">
+        <v>63803013</v>
+      </c>
+      <c r="C24" s="3"/>
+      <c r="D24" s="10">
+        <v>63794750</v>
+      </c>
+      <c r="E24" s="5">
+        <v>63986264</v>
+      </c>
+      <c r="F24" s="5">
+        <v>63782830</v>
+      </c>
+      <c r="G24" s="5">
+        <v>63950584</v>
+      </c>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="7">
+        <v>64023257</v>
+      </c>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" s="6">
+        <v>78.36</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="12">
+        <v>85.68</v>
+      </c>
+      <c r="E25" s="6">
+        <v>87.51</v>
+      </c>
+      <c r="F25" s="6">
+        <v>88.08</v>
+      </c>
+      <c r="G25" s="6">
+        <v>91.34</v>
+      </c>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="4">
+        <v>80.69</v>
+      </c>
+      <c r="K25" s="6"/>
+      <c r="L25" s="6"/>
+      <c r="M25" s="6"/>
+      <c r="N25" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C14CF4CA-8C99-EF45-943C-8F45564704CD}">
+  <dimension ref="A1:O25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="29.83203125" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="4">
+        <v>16</v>
+      </c>
+      <c r="G4" s="4">
+        <v>4</v>
+      </c>
+      <c r="H4" s="4">
+        <v>1</v>
+      </c>
+      <c r="I4" s="4">
+        <v>1</v>
+      </c>
+      <c r="J4" s="4">
+        <v>1</v>
+      </c>
+      <c r="K4" s="4">
+        <v>1</v>
+      </c>
+      <c r="L4" s="4">
+        <v>1</v>
+      </c>
+      <c r="M4" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="4">
+        <v>1</v>
+      </c>
+      <c r="C5" s="4">
+        <v>4</v>
+      </c>
+      <c r="D5" s="4">
+        <v>8</v>
+      </c>
+      <c r="E5" s="4">
+        <v>16</v>
+      </c>
+      <c r="F5" s="4">
+        <v>1</v>
+      </c>
+      <c r="G5" s="4">
+        <v>16</v>
+      </c>
+      <c r="H5" s="4">
+        <v>1</v>
+      </c>
+      <c r="I5" s="4">
+        <v>16</v>
+      </c>
+      <c r="J5" s="4">
+        <v>1</v>
+      </c>
+      <c r="K5" s="4">
+        <v>8</v>
+      </c>
+      <c r="L5" s="4">
+        <v>16</v>
+      </c>
+      <c r="M5" s="4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4">
+        <v>100</v>
+      </c>
+      <c r="C6" s="4">
+        <v>100</v>
+      </c>
+      <c r="D6" s="4">
+        <v>100</v>
+      </c>
+      <c r="E6" s="4">
+        <v>100</v>
+      </c>
+      <c r="F6" s="4">
+        <v>100</v>
+      </c>
+      <c r="G6" s="4">
+        <v>100</v>
+      </c>
+      <c r="H6" s="4">
+        <v>0</v>
+      </c>
+      <c r="I6" s="4">
+        <v>0</v>
+      </c>
+      <c r="J6" s="4">
+        <v>10</v>
+      </c>
+      <c r="K6" s="4">
+        <v>10</v>
+      </c>
+      <c r="L6" s="4">
+        <v>10</v>
+      </c>
+      <c r="M6" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" s="3"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="5">
+        <v>155193122250</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5">
+        <v>155193138800</v>
+      </c>
+      <c r="E8" s="5">
+        <v>155193120340</v>
+      </c>
+      <c r="F8" s="5">
+        <v>155193125490</v>
+      </c>
+      <c r="G8" s="5">
+        <v>155193125490</v>
+      </c>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="7">
+        <v>155193121730</v>
+      </c>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="5">
+        <v>366369</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5">
+        <v>366305</v>
+      </c>
+      <c r="E9" s="5">
+        <v>366433</v>
+      </c>
+      <c r="F9" s="5">
+        <v>547835</v>
+      </c>
+      <c r="G9" s="5">
+        <v>385027</v>
+      </c>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="7">
+        <v>368788</v>
+      </c>
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
@@ -3416,15 +4168,27 @@
       <c r="A11" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="5"/>
+      <c r="B11" s="5">
+        <v>2170</v>
+      </c>
       <c r="C11" s="5"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
+      <c r="D11" s="7">
+        <v>2206</v>
+      </c>
+      <c r="E11" s="5">
+        <v>2312</v>
+      </c>
+      <c r="F11" s="5">
+        <v>2148</v>
+      </c>
+      <c r="G11" s="5">
+        <v>2168</v>
+      </c>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
-      <c r="J11" s="4"/>
+      <c r="J11" s="4">
+        <v>2197</v>
+      </c>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
@@ -3435,15 +4199,27 @@
       <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="6"/>
+      <c r="B12" s="6">
+        <v>157</v>
+      </c>
       <c r="C12" s="4"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
+      <c r="D12" s="6">
+        <v>157</v>
+      </c>
+      <c r="E12" s="4">
+        <v>157</v>
+      </c>
+      <c r="F12" s="4">
+        <v>105</v>
+      </c>
+      <c r="G12" s="4">
+        <v>149</v>
+      </c>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
+      <c r="J12" s="4">
+        <v>156</v>
+      </c>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
@@ -3468,15 +4244,27 @@
       <c r="A14" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="5"/>
+      <c r="B14" s="5">
+        <v>57600925</v>
+      </c>
       <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
+      <c r="D14" s="5">
+        <v>57635159</v>
+      </c>
+      <c r="E14" s="5">
+        <v>57587494</v>
+      </c>
+      <c r="F14" s="5">
+        <v>57581609</v>
+      </c>
+      <c r="G14" s="5">
+        <v>57620846</v>
+      </c>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
-      <c r="J14" s="7"/>
+      <c r="J14" s="7">
+        <v>57627591</v>
+      </c>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
@@ -3487,15 +4275,27 @@
       <c r="A15" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="5"/>
+      <c r="B15" s="5">
+        <v>51068634</v>
+      </c>
       <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
+      <c r="D15" s="5">
+        <v>51097371</v>
+      </c>
+      <c r="E15" s="5">
+        <v>51031621</v>
+      </c>
+      <c r="F15" s="5">
+        <v>51075340</v>
+      </c>
+      <c r="G15" s="5">
+        <v>51070658</v>
+      </c>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
-      <c r="J15" s="7"/>
+      <c r="J15" s="7">
+        <v>5105891</v>
+      </c>
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
@@ -3506,15 +4306,27 @@
       <c r="A16" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="5"/>
+      <c r="B16" s="5">
+        <v>108669559</v>
+      </c>
       <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
+      <c r="D16" s="5">
+        <v>108732530</v>
+      </c>
+      <c r="E16" s="5">
+        <v>108619115</v>
+      </c>
+      <c r="F16" s="5">
+        <v>108656949</v>
+      </c>
+      <c r="G16" s="5">
+        <v>108691504</v>
+      </c>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
-      <c r="J16" s="7"/>
+      <c r="J16" s="7">
+        <v>62733482</v>
+      </c>
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
       <c r="M16" s="5"/>
@@ -3541,15 +4353,27 @@
       <c r="A18" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="5"/>
+      <c r="B18" s="5">
+        <v>108702327</v>
+      </c>
       <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
+      <c r="D18" s="5">
+        <v>108765298</v>
+      </c>
+      <c r="E18" s="5">
+        <v>108651883</v>
+      </c>
+      <c r="F18" s="5">
+        <v>108689717</v>
+      </c>
+      <c r="G18" s="5">
+        <v>108724272</v>
+      </c>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
-      <c r="J18" s="7"/>
+      <c r="J18" s="7">
+        <v>108731199</v>
+      </c>
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
       <c r="M18" s="5"/>
@@ -3560,15 +4384,27 @@
       <c r="A19" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="5"/>
+      <c r="B19" s="5">
+        <v>155084419930</v>
+      </c>
       <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
+      <c r="D19" s="5">
+        <v>155084373500</v>
+      </c>
+      <c r="E19" s="5">
+        <v>155084468460</v>
+      </c>
+      <c r="F19" s="5">
+        <v>155084435780</v>
+      </c>
+      <c r="G19" s="5">
+        <v>155084401220</v>
+      </c>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
-      <c r="J19" s="7"/>
+      <c r="J19" s="7">
+        <v>155084390530</v>
+      </c>
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
       <c r="M19" s="5"/>
@@ -3579,15 +4415,27 @@
       <c r="A20" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="5"/>
+      <c r="B20" s="5">
+        <v>107988801640</v>
+      </c>
       <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
+      <c r="D20" s="5">
+        <v>107988808690</v>
+      </c>
+      <c r="E20" s="5">
+        <v>107988800640</v>
+      </c>
+      <c r="F20" s="5">
+        <v>107988802030</v>
+      </c>
+      <c r="G20" s="5">
+        <v>107988802030</v>
+      </c>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
-      <c r="J20" s="7"/>
+      <c r="J20" s="7">
+        <v>107988801330</v>
+      </c>
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
       <c r="M20" s="5"/>
@@ -3598,15 +4446,27 @@
       <c r="A21" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B21" s="5"/>
+      <c r="B21" s="5">
+        <v>47204320618</v>
+      </c>
       <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
+      <c r="D21" s="5">
+        <v>47204330117</v>
+      </c>
+      <c r="E21" s="5">
+        <v>47204319702</v>
+      </c>
+      <c r="F21" s="5">
+        <v>47204323462</v>
+      </c>
+      <c r="G21" s="5">
+        <v>47204323462</v>
+      </c>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
-      <c r="J21" s="7"/>
+      <c r="J21" s="7">
+        <v>47204320396</v>
+      </c>
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
       <c r="M21" s="5"/>
@@ -3633,15 +4493,27 @@
       <c r="A23" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="5"/>
+      <c r="B23" s="5">
+        <v>57094544</v>
+      </c>
       <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
+      <c r="D23" s="5">
+        <v>59820540</v>
+      </c>
+      <c r="E23" s="5">
+        <v>60399215</v>
+      </c>
+      <c r="F23" s="5">
+        <v>62628471</v>
+      </c>
+      <c r="G23" s="5">
+        <v>65958453</v>
+      </c>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
-      <c r="J23" s="7"/>
+      <c r="J23" s="7">
+        <v>53340101</v>
+      </c>
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
       <c r="M23" s="5"/>
@@ -3652,15 +4524,27 @@
       <c r="A24" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="5"/>
+      <c r="B24" s="5">
+        <v>108702327</v>
+      </c>
       <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
+      <c r="D24" s="5">
+        <v>108765298</v>
+      </c>
+      <c r="E24" s="5">
+        <v>108651883</v>
+      </c>
+      <c r="F24" s="5">
+        <v>108689717</v>
+      </c>
+      <c r="G24" s="5">
+        <v>108724272</v>
+      </c>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
-      <c r="J24" s="7"/>
+      <c r="J24" s="7">
+        <v>108731199</v>
+      </c>
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
       <c r="M24" s="5"/>
@@ -3671,553 +4555,27 @@
       <c r="A25" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="6"/>
+      <c r="B25" s="6">
+        <v>52.52</v>
+      </c>
       <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
+      <c r="D25" s="6">
+        <v>55</v>
+      </c>
+      <c r="E25" s="6">
+        <v>55.59</v>
+      </c>
+      <c r="F25" s="6">
+        <v>57.62</v>
+      </c>
+      <c r="G25" s="6">
+        <v>60.67</v>
+      </c>
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>
-      <c r="J25" s="4"/>
-      <c r="K25" s="6"/>
-      <c r="L25" s="6"/>
-      <c r="M25" s="6"/>
-      <c r="N25" s="2"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C14CF4CA-8C99-EF45-943C-8F45564704CD}">
-  <dimension ref="A1:O25"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="29.83203125" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4">
-        <v>1</v>
-      </c>
-      <c r="C4" s="4">
-        <v>1</v>
-      </c>
-      <c r="D4" s="4">
-        <v>1</v>
-      </c>
-      <c r="E4" s="4">
-        <v>1</v>
-      </c>
-      <c r="F4" s="4">
-        <v>16</v>
-      </c>
-      <c r="G4" s="4">
-        <v>4</v>
-      </c>
-      <c r="H4" s="4">
-        <v>1</v>
-      </c>
-      <c r="I4" s="4">
-        <v>1</v>
-      </c>
-      <c r="J4" s="4">
-        <v>1</v>
-      </c>
-      <c r="K4" s="4">
-        <v>1</v>
-      </c>
-      <c r="L4" s="4">
-        <v>1</v>
-      </c>
-      <c r="M4" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="4">
-        <v>1</v>
-      </c>
-      <c r="C5" s="4">
-        <v>4</v>
-      </c>
-      <c r="D5" s="4">
-        <v>8</v>
-      </c>
-      <c r="E5" s="4">
-        <v>16</v>
-      </c>
-      <c r="F5" s="4">
-        <v>1</v>
-      </c>
-      <c r="G5" s="4">
-        <v>16</v>
-      </c>
-      <c r="H5" s="4">
-        <v>1</v>
-      </c>
-      <c r="I5" s="4">
-        <v>16</v>
-      </c>
-      <c r="J5" s="4">
-        <v>1</v>
-      </c>
-      <c r="K5" s="4">
-        <v>8</v>
-      </c>
-      <c r="L5" s="4">
-        <v>16</v>
-      </c>
-      <c r="M5" s="4">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="4">
-        <v>100</v>
-      </c>
-      <c r="C6" s="4">
-        <v>100</v>
-      </c>
-      <c r="D6" s="4">
-        <v>100</v>
-      </c>
-      <c r="E6" s="4">
-        <v>100</v>
-      </c>
-      <c r="F6" s="4">
-        <v>100</v>
-      </c>
-      <c r="G6" s="4">
-        <v>100</v>
-      </c>
-      <c r="H6" s="4">
-        <v>0</v>
-      </c>
-      <c r="I6" s="4">
-        <v>0</v>
-      </c>
-      <c r="J6" s="4">
-        <v>10</v>
-      </c>
-      <c r="K6" s="4">
-        <v>10</v>
-      </c>
-      <c r="L6" s="4">
-        <v>10</v>
-      </c>
-      <c r="M6" s="4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7" s="3"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="3"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13" s="3"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="1"/>
-      <c r="O15" s="1"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A17" s="3"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="1"/>
-      <c r="O17" s="1"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="1"/>
-      <c r="O18" s="1"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
-      <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A22" s="3"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="5"/>
-      <c r="N22" s="1"/>
-      <c r="O22" s="1"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
-      <c r="M23" s="5"/>
-      <c r="N23" s="1"/>
-      <c r="O23" s="1"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="5"/>
-      <c r="L24" s="5"/>
-      <c r="M24" s="5"/>
-      <c r="N24" s="1"/>
-      <c r="O24" s="1"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="4"/>
+      <c r="J25" s="4">
+        <v>49.06</v>
+      </c>
       <c r="K25" s="6"/>
       <c r="L25" s="6"/>
       <c r="M25" s="6"/>

</xml_diff>

<commit_message>
Updated results excel (x264 and leela v2)
</commit_message>
<xml_diff>
--- a/results/results_table.xlsx
+++ b/results/results_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max/Desktop/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{49DC639F-604F-A34A-9D80-939772D3C1BA}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{992EA1E1-622B-C049-BBA4-AFF78CEDFABB}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="4" xr2:uid="{4BDD7C24-A808-BD4F-9094-4693B707796C}"/>
   </bookViews>
@@ -229,9 +229,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -240,6 +237,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -568,15 +568,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
@@ -1442,15 +1442,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
@@ -2319,15 +2319,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
@@ -3183,7 +3183,7 @@
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+      <selection activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3193,15 +3193,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
@@ -3390,7 +3390,7 @@
         <v>107510874570</v>
       </c>
       <c r="C8" s="3"/>
-      <c r="D8" s="10">
+      <c r="D8" s="9">
         <v>107509988030</v>
       </c>
       <c r="E8" s="5">
@@ -3402,14 +3402,22 @@
       <c r="G8" s="5">
         <v>107509744320</v>
       </c>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
+      <c r="H8" s="5">
+        <v>107510278560</v>
+      </c>
+      <c r="I8" s="5">
+        <v>107510903140</v>
+      </c>
       <c r="J8" s="7">
         <v>107509744250</v>
       </c>
       <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
+      <c r="L8" s="5">
+        <v>107509988030</v>
+      </c>
+      <c r="M8" s="5">
+        <v>107510785740</v>
+      </c>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
     </row>
@@ -3421,7 +3429,7 @@
         <v>2439482</v>
       </c>
       <c r="C9" s="3"/>
-      <c r="D9" s="10">
+      <c r="D9" s="9">
         <v>2439481</v>
       </c>
       <c r="E9" s="5">
@@ -3433,14 +3441,22 @@
       <c r="G9" s="5">
         <v>2439480</v>
       </c>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
+      <c r="H9" s="5">
+        <v>2415441</v>
+      </c>
+      <c r="I9" s="5">
+        <v>2415441</v>
+      </c>
       <c r="J9" s="7">
         <v>2437132</v>
       </c>
       <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
+      <c r="L9" s="5">
+        <v>2437130</v>
+      </c>
+      <c r="M9" s="5">
+        <v>2437121</v>
+      </c>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
     </row>
@@ -3466,7 +3482,7 @@
         <v>477</v>
       </c>
       <c r="C11" s="3"/>
-      <c r="D11" s="11">
+      <c r="D11" s="10">
         <v>392</v>
       </c>
       <c r="E11" s="5">
@@ -3478,14 +3494,22 @@
       <c r="G11" s="5">
         <v>397</v>
       </c>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
+      <c r="H11" s="5">
+        <v>477</v>
+      </c>
+      <c r="I11" s="5">
+        <v>476</v>
+      </c>
       <c r="J11" s="5">
         <v>395</v>
       </c>
       <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
+      <c r="L11" s="5">
+        <v>395</v>
+      </c>
+      <c r="M11" s="5">
+        <v>481</v>
+      </c>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
     </row>
@@ -3497,7 +3521,7 @@
         <v>7</v>
       </c>
       <c r="C12" s="3"/>
-      <c r="D12" s="12">
+      <c r="D12" s="11">
         <v>7</v>
       </c>
       <c r="E12" s="4">
@@ -3509,14 +3533,22 @@
       <c r="G12" s="4">
         <v>7</v>
       </c>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
+      <c r="H12" s="4">
+        <v>7</v>
+      </c>
+      <c r="I12" s="4">
+        <v>7</v>
+      </c>
       <c r="J12" s="4">
         <v>7</v>
       </c>
       <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
+      <c r="L12" s="4">
+        <v>7</v>
+      </c>
+      <c r="M12" s="4">
+        <v>7</v>
+      </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
@@ -3542,7 +3574,7 @@
         <v>17092299</v>
       </c>
       <c r="C14" s="3"/>
-      <c r="D14" s="10">
+      <c r="D14" s="9">
         <v>17091385</v>
       </c>
       <c r="E14" s="5">
@@ -3554,14 +3586,22 @@
       <c r="G14" s="5">
         <v>17093773</v>
       </c>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
+      <c r="H14" s="5">
+        <v>17093812</v>
+      </c>
+      <c r="I14" s="5">
+        <v>17097377</v>
+      </c>
       <c r="J14" s="7">
         <v>17097085</v>
       </c>
       <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
+      <c r="L14" s="5">
+        <v>17093607</v>
+      </c>
+      <c r="M14" s="5">
+        <v>17095999</v>
+      </c>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
     </row>
@@ -3573,7 +3613,7 @@
         <v>46677946</v>
       </c>
       <c r="C15" s="3"/>
-      <c r="D15" s="10">
+      <c r="D15" s="9">
         <v>46670597</v>
       </c>
       <c r="E15" s="5">
@@ -3585,14 +3625,22 @@
       <c r="G15" s="5">
         <v>46824043</v>
       </c>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
+      <c r="H15" s="5">
+        <v>0</v>
+      </c>
+      <c r="I15" s="5">
+        <v>0</v>
+      </c>
       <c r="J15" s="7">
         <v>4689511</v>
       </c>
       <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
+      <c r="L15" s="5">
+        <v>4667133</v>
+      </c>
+      <c r="M15" s="5">
+        <v>4704936</v>
+      </c>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
     </row>
@@ -3604,7 +3652,7 @@
         <v>63770245</v>
       </c>
       <c r="C16" s="3"/>
-      <c r="D16" s="10">
+      <c r="D16" s="9">
         <v>63761982</v>
       </c>
       <c r="E16" s="5">
@@ -3616,14 +3664,22 @@
       <c r="G16" s="5">
         <v>63917816</v>
       </c>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
+      <c r="H16" s="5">
+        <v>17093812</v>
+      </c>
+      <c r="I16" s="5">
+        <v>17097377</v>
+      </c>
       <c r="J16" s="7">
         <v>21786596</v>
       </c>
       <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
+      <c r="L16" s="5">
+        <v>21760740</v>
+      </c>
+      <c r="M16" s="5">
+        <v>21800935</v>
+      </c>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
     </row>
@@ -3651,7 +3707,7 @@
         <v>63803013</v>
       </c>
       <c r="C18" s="3"/>
-      <c r="D18" s="10">
+      <c r="D18" s="9">
         <v>63794750</v>
       </c>
       <c r="E18" s="5">
@@ -3663,14 +3719,22 @@
       <c r="G18" s="5">
         <v>63950584</v>
       </c>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
+      <c r="H18" s="5">
+        <v>63974261</v>
+      </c>
+      <c r="I18" s="5">
+        <v>64135412</v>
+      </c>
       <c r="J18" s="7">
         <v>64023257</v>
       </c>
       <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
+      <c r="L18" s="5">
+        <v>63886577</v>
+      </c>
+      <c r="M18" s="5">
+        <v>64045624</v>
+      </c>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
     </row>
@@ -3682,7 +3746,7 @@
         <v>107447071560</v>
       </c>
       <c r="C19" s="3"/>
-      <c r="D19" s="10">
+      <c r="D19" s="9">
         <v>107446193280</v>
       </c>
       <c r="E19" s="5">
@@ -3694,14 +3758,22 @@
       <c r="G19" s="5">
         <v>107445793730</v>
       </c>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
+      <c r="H19" s="5">
+        <v>107446304300</v>
+      </c>
+      <c r="I19" s="5">
+        <v>107446767730</v>
+      </c>
       <c r="J19" s="7">
         <v>107445721000</v>
       </c>
       <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
+      <c r="L19" s="5">
+        <v>107446101460</v>
+      </c>
+      <c r="M19" s="5">
+        <v>107446740110</v>
+      </c>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
     </row>
@@ -3713,7 +3785,7 @@
         <v>86841438458</v>
       </c>
       <c r="C20" s="3"/>
-      <c r="D20" s="10">
+      <c r="D20" s="9">
         <v>86840995346</v>
       </c>
       <c r="E20" s="5">
@@ -3725,14 +3797,22 @@
       <c r="G20" s="5">
         <v>86840873487</v>
       </c>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
+      <c r="H20" s="5">
+        <v>86841140578</v>
+      </c>
+      <c r="I20" s="5">
+        <v>86841452900</v>
+      </c>
       <c r="J20" s="7">
         <v>86840873425</v>
       </c>
       <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
+      <c r="L20" s="5">
+        <v>86840995346</v>
+      </c>
+      <c r="M20" s="5">
+        <v>86841394041</v>
+      </c>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
     </row>
@@ -3744,7 +3824,7 @@
         <v>20669436113</v>
       </c>
       <c r="C21" s="3"/>
-      <c r="D21" s="10">
+      <c r="D21" s="9">
         <v>20668992688</v>
       </c>
       <c r="E21" s="5">
@@ -3756,14 +3836,22 @@
       <c r="G21" s="5">
         <v>20668870829</v>
       </c>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
+      <c r="H21" s="5">
+        <v>20669137985</v>
+      </c>
+      <c r="I21" s="5">
+        <v>20669450242</v>
+      </c>
       <c r="J21" s="7">
         <v>20668870829</v>
       </c>
       <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
+      <c r="L21" s="5">
+        <v>20668992688</v>
+      </c>
+      <c r="M21" s="5">
+        <v>20669391696</v>
+      </c>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
     </row>
@@ -3791,7 +3879,7 @@
         <v>49998363</v>
       </c>
       <c r="C23" s="3"/>
-      <c r="D23" s="10">
+      <c r="D23" s="9">
         <v>54659042</v>
       </c>
       <c r="E23" s="5">
@@ -3803,14 +3891,22 @@
       <c r="G23" s="5">
         <v>58411091</v>
       </c>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
+      <c r="H23" s="5">
+        <v>51368489</v>
+      </c>
+      <c r="I23" s="5">
+        <v>60119542</v>
+      </c>
       <c r="J23" s="7">
         <v>51663151</v>
       </c>
       <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
-      <c r="M23" s="5"/>
+      <c r="L23" s="5">
+        <v>58933089</v>
+      </c>
+      <c r="M23" s="5">
+        <v>60562719</v>
+      </c>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
     </row>
@@ -3822,7 +3918,7 @@
         <v>63803013</v>
       </c>
       <c r="C24" s="3"/>
-      <c r="D24" s="10">
+      <c r="D24" s="9">
         <v>63794750</v>
       </c>
       <c r="E24" s="5">
@@ -3834,14 +3930,22 @@
       <c r="G24" s="5">
         <v>63950584</v>
       </c>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
+      <c r="H24" s="5">
+        <v>63974261</v>
+      </c>
+      <c r="I24" s="5">
+        <v>64135412</v>
+      </c>
       <c r="J24" s="7">
         <v>64023257</v>
       </c>
       <c r="K24" s="5"/>
-      <c r="L24" s="5"/>
-      <c r="M24" s="5"/>
+      <c r="L24" s="5">
+        <v>63886577</v>
+      </c>
+      <c r="M24" s="5">
+        <v>64045624</v>
+      </c>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
     </row>
@@ -3853,7 +3957,7 @@
         <v>78.36</v>
       </c>
       <c r="C25" s="3"/>
-      <c r="D25" s="12">
+      <c r="D25" s="11">
         <v>85.68</v>
       </c>
       <c r="E25" s="6">
@@ -3865,14 +3969,22 @@
       <c r="G25" s="6">
         <v>91.34</v>
       </c>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
+      <c r="H25" s="6">
+        <v>80.3</v>
+      </c>
+      <c r="I25" s="6">
+        <v>93.74</v>
+      </c>
       <c r="J25" s="4">
         <v>80.69</v>
       </c>
       <c r="K25" s="6"/>
-      <c r="L25" s="6"/>
-      <c r="M25" s="6"/>
+      <c r="L25" s="6">
+        <v>92.25</v>
+      </c>
+      <c r="M25" s="6">
+        <v>94.56</v>
+      </c>
       <c r="N25" s="2"/>
     </row>
   </sheetData>
@@ -3889,7 +4001,7 @@
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3899,15 +4011,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
@@ -4108,14 +4220,22 @@
       <c r="G8" s="5">
         <v>155193125490</v>
       </c>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
+      <c r="H8" s="5">
+        <v>155193124280</v>
+      </c>
+      <c r="I8" s="5">
+        <v>155193120970</v>
+      </c>
       <c r="J8" s="7">
         <v>155193121730</v>
       </c>
       <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
+      <c r="L8" s="5">
+        <v>155193120340</v>
+      </c>
+      <c r="M8" s="5">
+        <v>155193120460</v>
+      </c>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
     </row>
@@ -4139,14 +4259,22 @@
       <c r="G9" s="5">
         <v>385027</v>
       </c>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
+      <c r="H9" s="5">
+        <v>367476</v>
+      </c>
+      <c r="I9" s="5">
+        <v>367604</v>
+      </c>
       <c r="J9" s="7">
         <v>368788</v>
       </c>
       <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
+      <c r="L9" s="5">
+        <v>369041</v>
+      </c>
+      <c r="M9" s="5">
+        <v>357775</v>
+      </c>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
     </row>
@@ -4184,14 +4312,22 @@
       <c r="G11" s="5">
         <v>2168</v>
       </c>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
+      <c r="H11" s="5">
+        <v>2294</v>
+      </c>
+      <c r="I11" s="5">
+        <v>2246</v>
+      </c>
       <c r="J11" s="4">
         <v>2197</v>
       </c>
       <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
+      <c r="L11" s="5">
+        <v>2198</v>
+      </c>
+      <c r="M11" s="5">
+        <v>2312</v>
+      </c>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
     </row>
@@ -4215,14 +4351,22 @@
       <c r="G12" s="4">
         <v>149</v>
       </c>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
+      <c r="H12" s="4">
+        <v>156</v>
+      </c>
+      <c r="I12" s="4">
+        <v>156</v>
+      </c>
       <c r="J12" s="4">
         <v>156</v>
       </c>
       <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
+      <c r="L12" s="4">
+        <v>156</v>
+      </c>
+      <c r="M12" s="4">
+        <v>161</v>
+      </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
@@ -4260,14 +4404,22 @@
       <c r="G14" s="5">
         <v>57620846</v>
       </c>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
+      <c r="H14" s="5">
+        <v>57600695</v>
+      </c>
+      <c r="I14" s="5">
+        <v>57586284</v>
+      </c>
       <c r="J14" s="7">
         <v>57627591</v>
       </c>
       <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
+      <c r="L14" s="5">
+        <v>57574063</v>
+      </c>
+      <c r="M14" s="5">
+        <v>57645024</v>
+      </c>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
     </row>
@@ -4291,14 +4443,22 @@
       <c r="G15" s="5">
         <v>51070658</v>
       </c>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
+      <c r="H15" s="5">
+        <v>0</v>
+      </c>
+      <c r="I15" s="5">
+        <v>0</v>
+      </c>
       <c r="J15" s="7">
         <v>5105891</v>
       </c>
       <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
+      <c r="L15" s="5">
+        <v>5106126</v>
+      </c>
+      <c r="M15" s="5">
+        <v>5108863</v>
+      </c>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
     </row>
@@ -4322,14 +4482,22 @@
       <c r="G16" s="5">
         <v>108691504</v>
       </c>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
+      <c r="H16" s="5">
+        <v>57600695</v>
+      </c>
+      <c r="I16" s="5">
+        <v>57586284</v>
+      </c>
       <c r="J16" s="7">
         <v>62733482</v>
       </c>
       <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
+      <c r="L16" s="5">
+        <v>62680189</v>
+      </c>
+      <c r="M16" s="5">
+        <v>62753887</v>
+      </c>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
     </row>
@@ -4369,14 +4537,22 @@
       <c r="G18" s="5">
         <v>108724272</v>
       </c>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
+      <c r="H18" s="5">
+        <v>108680035</v>
+      </c>
+      <c r="I18" s="5">
+        <v>108670799</v>
+      </c>
       <c r="J18" s="7">
         <v>108731199</v>
       </c>
       <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
+      <c r="L18" s="5">
+        <v>108663658</v>
+      </c>
+      <c r="M18" s="5">
+        <v>108756298</v>
+      </c>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
     </row>
@@ -4400,14 +4576,22 @@
       <c r="G19" s="5">
         <v>155084401220</v>
       </c>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
+      <c r="H19" s="5">
+        <v>155084444250</v>
+      </c>
+      <c r="I19" s="5">
+        <v>155084450170</v>
+      </c>
       <c r="J19" s="7">
         <v>155084390530</v>
       </c>
       <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
+      <c r="L19" s="5">
+        <v>155084456680</v>
+      </c>
+      <c r="M19" s="5">
+        <v>155084364160</v>
+      </c>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
     </row>
@@ -4431,14 +4615,22 @@
       <c r="G20" s="5">
         <v>107988802030</v>
       </c>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
+      <c r="H20" s="5">
+        <v>107988801430</v>
+      </c>
+      <c r="I20" s="5">
+        <v>107988801000</v>
+      </c>
       <c r="J20" s="7">
         <v>107988801330</v>
       </c>
       <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
+      <c r="L20" s="5">
+        <v>107988800640</v>
+      </c>
+      <c r="M20" s="5">
+        <v>107988801170</v>
+      </c>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
     </row>
@@ -4462,14 +4654,22 @@
       <c r="G21" s="5">
         <v>47204323462</v>
       </c>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
+      <c r="H21" s="5">
+        <v>47204322858</v>
+      </c>
+      <c r="I21" s="5">
+        <v>47204319978</v>
+      </c>
       <c r="J21" s="7">
         <v>47204320396</v>
       </c>
       <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
+      <c r="L21" s="5">
+        <v>47204319702</v>
+      </c>
+      <c r="M21" s="5">
+        <v>47204319288</v>
+      </c>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
     </row>
@@ -4509,14 +4709,22 @@
       <c r="G23" s="5">
         <v>65958453</v>
       </c>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
+      <c r="H23" s="5">
+        <v>52846938</v>
+      </c>
+      <c r="I23" s="5">
+        <v>57592203</v>
+      </c>
       <c r="J23" s="7">
         <v>53340101</v>
       </c>
       <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
-      <c r="M23" s="5"/>
+      <c r="L23" s="5">
+        <v>70960177</v>
+      </c>
+      <c r="M23" s="5">
+        <v>77219635</v>
+      </c>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
     </row>
@@ -4540,14 +4748,22 @@
       <c r="G24" s="5">
         <v>108724272</v>
       </c>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
+      <c r="H24" s="5">
+        <v>108680035</v>
+      </c>
+      <c r="I24" s="5">
+        <v>108670799</v>
+      </c>
       <c r="J24" s="7">
         <v>108731199</v>
       </c>
       <c r="K24" s="5"/>
-      <c r="L24" s="5"/>
-      <c r="M24" s="5"/>
+      <c r="L24" s="5">
+        <v>108663658</v>
+      </c>
+      <c r="M24" s="5">
+        <v>108756298</v>
+      </c>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
     </row>
@@ -4571,14 +4787,22 @@
       <c r="G25" s="6">
         <v>60.67</v>
       </c>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
+      <c r="H25" s="6">
+        <v>48.63</v>
+      </c>
+      <c r="I25" s="6">
+        <v>53</v>
+      </c>
       <c r="J25" s="4">
         <v>49.06</v>
       </c>
       <c r="K25" s="6"/>
-      <c r="L25" s="6"/>
-      <c r="M25" s="6"/>
+      <c r="L25" s="6">
+        <v>65.3</v>
+      </c>
+      <c r="M25" s="6">
+        <v>71</v>
+      </c>
       <c r="N25" s="2"/>
     </row>
   </sheetData>

</xml_diff>